<commit_message>
March 2023 data update
</commit_message>
<xml_diff>
--- a/Data/Excel_Long/camino_ages_long.xlsx
+++ b/Data/Excel_Long/camino_ages_long.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F677"/>
+  <dimension ref="A1:F680"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16684,6 +16684,78 @@
         <v>198</v>
       </c>
     </row>
+    <row r="678">
+      <c r="A678" s="1" t="n">
+        <v>676</v>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>202302</t>
+        </is>
+      </c>
+      <c r="C678" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D678" t="n">
+        <v>2</v>
+      </c>
+      <c r="E678" t="inlineStr">
+        <is>
+          <t>30-60</t>
+        </is>
+      </c>
+      <c r="F678" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" s="1" t="n">
+        <v>677</v>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>202302</t>
+        </is>
+      </c>
+      <c r="C679" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D679" t="n">
+        <v>2</v>
+      </c>
+      <c r="E679" t="inlineStr">
+        <is>
+          <t>&lt;30</t>
+        </is>
+      </c>
+      <c r="F679" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" s="1" t="n">
+        <v>678</v>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>202302</t>
+        </is>
+      </c>
+      <c r="C680" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D680" t="n">
+        <v>2</v>
+      </c>
+      <c r="E680" t="inlineStr">
+        <is>
+          <t>&gt;60</t>
+        </is>
+      </c>
+      <c r="F680" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>